<commit_message>
Fixed Feign Relations Finder and added 7 projects.
</commit_message>
<xml_diff>
--- a/data/Andante/activity-client_structure.xlsx
+++ b/data/Andante/activity-client_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3025" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="273">
   <si>
     <t>Class Name</t>
   </si>
@@ -8011,7 +8011,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8099,10 +8099,10 @@
         <v>46</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9">
@@ -8110,7 +8110,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>264</v>
@@ -8121,10 +8121,10 @@
         <v>46</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11">
@@ -8132,7 +8132,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>265</v>
@@ -8143,7 +8143,7 @@
         <v>46</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>265</v>
@@ -8151,13 +8151,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>265</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14">
@@ -8165,10 +8165,10 @@
         <v>65</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15">
@@ -8176,7 +8176,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>266</v>
@@ -8187,7 +8187,7 @@
         <v>65</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>266</v>
@@ -8198,10 +8198,10 @@
         <v>65</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18">
@@ -8209,7 +8209,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>264</v>
@@ -8217,10 +8217,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>264</v>
@@ -8231,21 +8231,21 @@
         <v>72</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22">
@@ -8253,10 +8253,10 @@
         <v>75</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23">
@@ -8264,7 +8264,7 @@
         <v>75</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>266</v>
@@ -8275,7 +8275,7 @@
         <v>75</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>266</v>
@@ -8286,7 +8286,7 @@
         <v>75</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>266</v>
@@ -8297,10 +8297,10 @@
         <v>75</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27">
@@ -8308,18 +8308,18 @@
         <v>75</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>264</v>
@@ -8327,10 +8327,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>264</v>
@@ -8341,7 +8341,7 @@
         <v>83</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>264</v>
@@ -8352,7 +8352,7 @@
         <v>83</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>264</v>
@@ -8363,7 +8363,7 @@
         <v>83</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>264</v>
@@ -8374,7 +8374,7 @@
         <v>83</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>264</v>
@@ -8385,7 +8385,7 @@
         <v>83</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s" s="0">
         <v>264</v>
@@ -8396,10 +8396,10 @@
         <v>83</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36">
@@ -8407,7 +8407,7 @@
         <v>83</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>264</v>
@@ -8418,10 +8418,10 @@
         <v>83</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38">
@@ -8429,7 +8429,7 @@
         <v>83</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s" s="0">
         <v>264</v>
@@ -8440,10 +8440,10 @@
         <v>83</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40">
@@ -8451,29 +8451,29 @@
         <v>83</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>242</v>
@@ -8481,24 +8481,24 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="45">
@@ -8506,10 +8506,10 @@
         <v>99</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46">
@@ -8517,10 +8517,10 @@
         <v>99</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47">
@@ -8528,32 +8528,32 @@
         <v>99</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50">
@@ -8561,10 +8561,10 @@
         <v>102</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51">
@@ -8572,7 +8572,7 @@
         <v>102</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>266</v>
@@ -8583,7 +8583,7 @@
         <v>102</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>266</v>
@@ -8594,7 +8594,7 @@
         <v>102</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>266</v>
@@ -8605,7 +8605,7 @@
         <v>102</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C54" t="s" s="0">
         <v>266</v>
@@ -8616,7 +8616,7 @@
         <v>102</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s" s="0">
         <v>266</v>
@@ -8627,7 +8627,7 @@
         <v>102</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s" s="0">
         <v>266</v>
@@ -8638,7 +8638,7 @@
         <v>102</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s" s="0">
         <v>266</v>
@@ -8649,7 +8649,7 @@
         <v>102</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s" s="0">
         <v>266</v>
@@ -8660,7 +8660,7 @@
         <v>102</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s" s="0">
         <v>266</v>
@@ -8671,10 +8671,10 @@
         <v>102</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61">
@@ -8682,32 +8682,32 @@
         <v>102</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64">
@@ -8715,10 +8715,10 @@
         <v>94</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65">
@@ -8726,7 +8726,7 @@
         <v>94</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s" s="0">
         <v>266</v>
@@ -8737,10 +8737,10 @@
         <v>94</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67">
@@ -8748,18 +8748,18 @@
         <v>94</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s" s="0">
         <v>264</v>
@@ -8767,13 +8767,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70">
@@ -9009,10 +9009,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="0">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>264</v>
@@ -9020,13 +9020,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="0">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>242</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93">
@@ -9034,7 +9034,7 @@
         <v>132</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>264</v>
@@ -9045,7 +9045,7 @@
         <v>132</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>264</v>
@@ -9056,7 +9056,7 @@
         <v>132</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="C95" t="s" s="0">
         <v>264</v>
@@ -9067,7 +9067,7 @@
         <v>132</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C96" t="s" s="0">
         <v>264</v>
@@ -9078,7 +9078,7 @@
         <v>132</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C97" t="s" s="0">
         <v>264</v>
@@ -9089,7 +9089,7 @@
         <v>132</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>264</v>
@@ -9100,7 +9100,7 @@
         <v>132</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C99" t="s" s="0">
         <v>264</v>
@@ -9111,10 +9111,10 @@
         <v>132</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="101">
@@ -9122,32 +9122,32 @@
         <v>132</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s" s="0">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s" s="0">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="0">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>242</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104">
@@ -9155,7 +9155,7 @@
         <v>101</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="C104" t="s" s="0">
         <v>264</v>
@@ -9166,10 +9166,10 @@
         <v>101</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="106">
@@ -9177,10 +9177,10 @@
         <v>101</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107">
@@ -9408,10 +9408,10 @@
         <v>78</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="128">
@@ -9419,7 +9419,7 @@
         <v>78</v>
       </c>
       <c r="B128" t="s" s="0">
-        <v>185</v>
+        <v>93</v>
       </c>
       <c r="C128" t="s" s="0">
         <v>264</v>
@@ -9430,7 +9430,7 @@
         <v>78</v>
       </c>
       <c r="B129" t="s" s="0">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="C129" t="s" s="0">
         <v>264</v>
@@ -9441,7 +9441,7 @@
         <v>78</v>
       </c>
       <c r="B130" t="s" s="0">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C130" t="s" s="0">
         <v>264</v>
@@ -9452,7 +9452,7 @@
         <v>78</v>
       </c>
       <c r="B131" t="s" s="0">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="C131" t="s" s="0">
         <v>264</v>
@@ -9463,7 +9463,7 @@
         <v>78</v>
       </c>
       <c r="B132" t="s" s="0">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C132" t="s" s="0">
         <v>264</v>
@@ -9474,7 +9474,7 @@
         <v>78</v>
       </c>
       <c r="B133" t="s" s="0">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C133" t="s" s="0">
         <v>264</v>
@@ -9485,7 +9485,7 @@
         <v>78</v>
       </c>
       <c r="B134" t="s" s="0">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C134" t="s" s="0">
         <v>264</v>
@@ -9496,7 +9496,7 @@
         <v>78</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C135" t="s" s="0">
         <v>264</v>
@@ -9507,7 +9507,7 @@
         <v>78</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C136" t="s" s="0">
         <v>264</v>
@@ -9518,7 +9518,7 @@
         <v>78</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C137" t="s" s="0">
         <v>264</v>
@@ -9529,10 +9529,10 @@
         <v>78</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="139">
@@ -9540,10 +9540,10 @@
         <v>78</v>
       </c>
       <c r="B139" t="s" s="0">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140">
@@ -9551,10 +9551,10 @@
         <v>78</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="141">
@@ -9562,10 +9562,43 @@
         <v>78</v>
       </c>
       <c r="B141" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s" s="0">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B142" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="C141" t="s" s="0">
+      <c r="C142" t="s" s="0">
         <v>264</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="B143" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="C143" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="B144" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="C144" t="s" s="0">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>